<commit_message>
agrego validación en pantalla de informacion basica para cargar telefono y mail si no los tiene
</commit_message>
<xml_diff>
--- a/SuraClaims/DataSource - Ambiente y Usuario.xlsx
+++ b/SuraClaims/DataSource - Ambiente y Usuario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A413A3-AFE2-4778-A74F-7F7AA2ACE2AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B70FB3D-59A6-4411-AF0C-76F316C2D334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DD4D5B32-3ED0-4AA2-B8F8-538A2E83AD60}"/>
   </bookViews>
@@ -51,13 +51,13 @@
     <t>gw</t>
   </si>
   <si>
-    <t>https://i-preproducciongestion.segurossura.com.ar/cc/ClaimCenter.do</t>
-  </si>
-  <si>
-    <t>i-preproducciongestion.segurossura.com.ar</t>
-  </si>
-  <si>
     <t>silverarrow</t>
+  </si>
+  <si>
+    <t>preproducciongestion.segurossura.com.ar</t>
+  </si>
+  <si>
+    <t>https://preproducciongestion.segurossura.com.ar/cc/ClaimCenter.do</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,13 +461,13 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>